<commit_message>
Replace urls in metadata
</commit_message>
<xml_diff>
--- a/automation/abstimmungsergebnisse/politik_abstimmungen_seit1933_metadata.xlsx
+++ b/automation/abstimmungsergebnisse/politik_abstimmungen_seit1933_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sszgua\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sszgua\Python\git\opendatazurich.github.io\automation\abstimmungsergebnisse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAB0A32-BF82-4CD8-A70C-EC8BD4157C67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413F4F1E-890D-4BCD-9A2E-FB6AE842C823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1065" yWindow="-120" windowWidth="27855" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -706,7 +706,7 @@
   </si>
   <si>
     <t xml:space="preserve">Enthält die Resultate aller Abstimmungen seit 1933 auf kommunaler, kantonaler und eidgenössischer Ebene.
-Die Abstimmungsresultate werden von Statistik Stadt Zürich in der sog. **Abstimmungsdatenbank** erfasst und sind im Internet unter [**diesem Link**](https://www.stadt-zuerich.ch/prd/de/index/statistik/themen/staat-recht-politik/politik/abstimmungen.html) zugänglich. 
+Die Abstimmungsresultate werden von Statistik Stadt Zürich in der sog. **Abstimmungsdatenbank** erfasst und sind im Internet unter [**diesem Link**](https://www.stadt-zuerich.ch/de/politik-und-verwaltung/statistik-und-daten/daten/politik-und-verwaltung/politik/abstimmungen.html) zugänglich. 
 </t>
   </si>
 </sst>
@@ -1326,7 +1326,7 @@
   <dimension ref="A1:G68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="255.5" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Adjustments to column names for R Shiny App
</commit_message>
<xml_diff>
--- a/automation/abstimmungsergebnisse/politik_abstimmungen_seit1933_metadata.xlsx
+++ b/automation/abstimmungsergebnisse/politik_abstimmungen_seit1933_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sszgua\Python\git\opendatazurich.github.io\automation\abstimmungsergebnisse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413F4F1E-890D-4BCD-9A2E-FB6AE842C823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A15A4A26-7970-4AA3-AD27-7D5013D79D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1065" yWindow="-120" windowWidth="27855" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24600" yWindow="-7785" windowWidth="28110" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="244">
   <si>
     <t>Tagname</t>
   </si>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t>Kategorie</t>
-  </si>
-  <si>
-    <t>Politik</t>
   </si>
   <si>
     <t>1-n Angaben aus den Werten des Sheets kategorien_werteliste.  z.B. Umwelt, Bevölkerung</t>
@@ -372,60 +369,39 @@
     <t>Anzahl stimmberechtigter Personen zum Zeitpunkt der Abstimmung</t>
   </si>
   <si>
-    <t>Ja</t>
-  </si>
-  <si>
     <t>Ja-Stimmen</t>
   </si>
   <si>
     <t>Anzahl Ja-Stimmen</t>
   </si>
   <si>
-    <t>Nein</t>
-  </si>
-  <si>
     <t>Nein-Stimmen</t>
   </si>
   <si>
     <t>Anzahl Nein-Stimmen</t>
   </si>
   <si>
-    <t>Stimmbeteiligung (%)</t>
-  </si>
-  <si>
     <t>Stimmbeteiligung in Prozent</t>
   </si>
   <si>
-    <t>Ja (%)</t>
-  </si>
-  <si>
     <t>Ja-Anteil in Prozent</t>
   </si>
   <si>
     <t>Prozentualer Anteil Ja-Stimmen</t>
   </si>
   <si>
-    <t>Nein (%)</t>
-  </si>
-  <si>
     <t>Nein-Anteil in Prozent</t>
   </si>
   <si>
     <t>Prozentualer Anteil Nein-Stimmen</t>
   </si>
   <si>
-    <t>StaendeJa</t>
-  </si>
-  <si>
     <t>Ja-Stände</t>
   </si>
   <si>
     <t>Anzahl Stände Ja</t>
   </si>
   <si>
-    <t>SteandeNein</t>
-  </si>
-  <si>
     <t>Nein-Stände</t>
   </si>
   <si>
@@ -706,8 +682,89 @@
   </si>
   <si>
     <t xml:space="preserve">Enthält die Resultate aller Abstimmungen seit 1933 auf kommunaler, kantonaler und eidgenössischer Ebene.
-Die Abstimmungsresultate werden von Statistik Stadt Zürich in der sog. **Abstimmungsdatenbank** erfasst und sind im Internet unter [**diesem Link**](https://www.stadt-zuerich.ch/de/politik-und-verwaltung/statistik-und-daten/daten/politik-und-verwaltung/politik/abstimmungen.html) zugänglich. 
+Die Abstimmungsresultate werden von Statistik Stadt Zürich in der sog. **Abstimmungsdatenbank** erfasst und sind im Internet unter [**diesem Link**](https://www.stadt-zuerich.ch/prd/de/index/statistik/themen/staat-recht-politik/politik/abstimmungen.html) zugänglich. 
 </t>
+  </si>
+  <si>
+    <t>Stimmbeteiligung_Prozent</t>
+  </si>
+  <si>
+    <t>Nein_Prozent</t>
+  </si>
+  <si>
+    <t>Ja_Prozent</t>
+  </si>
+  <si>
+    <t>Ja_Absolut</t>
+  </si>
+  <si>
+    <t>Nein_Absolut</t>
+  </si>
+  <si>
+    <t>Staende_Ja</t>
+  </si>
+  <si>
+    <t>Staende_Nein</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>arbeit-und-erwerb</t>
+  </si>
+  <si>
+    <t>basiskarten,</t>
+  </si>
+  <si>
+    <t>bauen-und-wohnen</t>
+  </si>
+  <si>
+    <t>bevolkerung</t>
+  </si>
+  <si>
+    <t>bildung</t>
+  </si>
+  <si>
+    <t>energie</t>
+  </si>
+  <si>
+    <t>finanzen</t>
+  </si>
+  <si>
+    <t>freizeit</t>
+  </si>
+  <si>
+    <t>gesundheit</t>
+  </si>
+  <si>
+    <t>kriminalitat</t>
+  </si>
+  <si>
+    <t>kultur</t>
+  </si>
+  <si>
+    <t>mobilitat</t>
+  </si>
+  <si>
+    <t>politik</t>
+  </si>
+  <si>
+    <t>preise</t>
+  </si>
+  <si>
+    <t>soziales</t>
+  </si>
+  <si>
+    <t>tourismus</t>
+  </si>
+  <si>
+    <t>umwelt</t>
+  </si>
+  <si>
+    <t>verwaltung</t>
+  </si>
+  <si>
+    <t>volkswirtschaft</t>
   </si>
 </sst>
 </file>
@@ -717,13 +774,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -964,22 +1027,19 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -994,84 +1054,93 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="14" fontId="15" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="16" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="6" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1326,7 +1395,7 @@
   <dimension ref="A1:G68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="255.5" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1394,7 +1463,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="8" t="s">
@@ -1412,243 +1481,243 @@
         <v>9</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>17</v>
+        <v>237</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="4" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="C5" s="17" t="s">
         <v>20</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>21</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="7"/>
       <c r="F5" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>23</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>24</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="4" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="14" t="s">
         <v>27</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>28</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>31</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>32</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="14" t="s">
         <v>35</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>36</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="C10" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="18" t="s">
         <v>40</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>41</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="C11" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="19" t="s">
         <v>44</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>45</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="C12" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="19" t="s">
         <v>48</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>49</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="14" t="s">
         <v>51</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>52</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>55</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>56</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="14" t="s">
         <v>59</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>60</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="C16" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="20" t="s">
         <v>64</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>65</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="C17" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="20" t="s">
         <v>68</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>69</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -1660,13 +1729,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="9" t="s">
-        <v>72</v>
-      </c>
       <c r="C19" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
@@ -1676,32 +1745,32 @@
         <v>8</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="B21" s="21" t="s">
+      <c r="C21" s="21" t="s">
         <v>74</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="42.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B22" s="21"/>
       <c r="C22" s="21"/>
       <c r="D22" s="1"/>
       <c r="E22" s="7"/>
       <c r="F22" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
@@ -1710,7 +1779,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="7"/>
       <c r="F23" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1735,10 +1804,10 @@
     </row>
     <row r="27" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" s="9" t="s">
         <v>78</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>79</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>9</v>
@@ -1746,288 +1815,288 @@
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
       <c r="B28" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="D28" s="13" t="s">
         <v>82</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>83</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="B29" s="21" t="s">
+      <c r="C29" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="C29" s="21" t="s">
+      <c r="D29" s="21" t="s">
         <v>87</v>
-      </c>
-      <c r="D29" s="21" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B30" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="D30" s="21" t="s">
         <v>90</v>
-      </c>
-      <c r="D30" s="21" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B31" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="C31" s="21" t="s">
+      <c r="D31" s="21" t="s">
         <v>93</v>
-      </c>
-      <c r="D31" s="21" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B32" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="D32" s="21" t="s">
         <v>96</v>
-      </c>
-      <c r="D32" s="21" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B33" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="C33" s="21" t="s">
+      <c r="D33" s="21" t="s">
         <v>99</v>
-      </c>
-      <c r="D33" s="21" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B34" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C34" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="C34" s="21" t="s">
+      <c r="D34" s="21" t="s">
         <v>102</v>
-      </c>
-      <c r="D34" s="21" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B35" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="C35" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="C35" s="21" t="s">
+      <c r="D35" s="21" t="s">
         <v>105</v>
-      </c>
-      <c r="D35" s="21" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B36" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="C36" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="C36" s="21" t="s">
+      <c r="D36" s="21" t="s">
         <v>108</v>
-      </c>
-      <c r="D36" s="21" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B37" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="C37" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="C37" s="21" t="s">
+      <c r="D37" s="21" t="s">
         <v>111</v>
-      </c>
-      <c r="D37" s="21" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B38" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="D38" s="21" t="s">
         <v>113</v>
-      </c>
-      <c r="C38" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="D38" s="21" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>116</v>
+        <v>221</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D39" s="21" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>119</v>
+        <v>217</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>121</v>
+        <v>219</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D41" s="21" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>124</v>
+        <v>218</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D42" s="21" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>127</v>
+        <v>222</v>
       </c>
       <c r="C43" s="21" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D43" s="21" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>130</v>
+        <v>223</v>
       </c>
       <c r="C44" s="21" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="45" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B45" s="21"/>
       <c r="C45" s="21"/>
       <c r="D45" s="21"/>
       <c r="E45" s="7"/>
       <c r="F45" s="4" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B46" s="21"/>
       <c r="C46" s="21"/>
       <c r="D46" s="21"/>
       <c r="E46" s="7"/>
       <c r="F46" s="4" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B47" s="21"/>
       <c r="C47" s="21"/>
       <c r="D47" s="21"/>
       <c r="E47" s="7"/>
       <c r="F47" s="4" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B48" s="21"/>
       <c r="C48" s="21"/>
@@ -2036,7 +2105,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B49" s="21"/>
       <c r="C49" s="21"/>
@@ -2045,7 +2114,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B50" s="21"/>
       <c r="C50" s="21"/>
@@ -2054,7 +2123,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B51" s="21"/>
       <c r="C51" s="21"/>
@@ -2063,7 +2132,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B52" s="21"/>
       <c r="C52" s="21"/>
@@ -2072,7 +2141,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B53" s="21"/>
       <c r="C53" s="21"/>
@@ -2081,7 +2150,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B54" s="21"/>
       <c r="C54" s="21"/>
@@ -2090,7 +2159,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B55" s="21"/>
       <c r="C55" s="21"/>
@@ -2099,7 +2168,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B56" s="21"/>
       <c r="C56" s="21"/>
@@ -2108,7 +2177,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B57" s="21"/>
       <c r="C57" s="21"/>
@@ -2117,7 +2186,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B58" s="21"/>
       <c r="C58" s="21"/>
@@ -2144,7 +2213,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B62" s="3" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="7"/>
@@ -2158,13 +2227,13 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D64" s="6"/>
       <c r="E64" s="6"/>
@@ -2172,7 +2241,7 @@
     </row>
     <row r="65" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B65" s="13" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="C65" s="13" t="s">
         <v>12</v>
@@ -2180,12 +2249,12 @@
       <c r="D65" s="13"/>
       <c r="E65" s="7"/>
       <c r="F65" s="8" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="11" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B66" s="12"/>
       <c r="C66" s="12"/>
@@ -2195,7 +2264,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="11" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B67" s="12"/>
       <c r="C67" s="12"/>
@@ -2218,10 +2287,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A24"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2244,114 +2313,174 @@
     <col min="16" max="16384" width="11" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" s="36" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" s="36" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" s="35" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="29" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
+      <c r="B9" s="35" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="29" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
+      <c r="B10" s="35" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="29" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="29" t="s">
+      <c r="B11" s="35" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="29" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="29" t="s">
+      <c r="B12" s="35" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="29" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="29" t="s">
+      <c r="B13" s="35" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="29" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="29" t="s">
+      <c r="B14" s="35" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="29" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="29" t="s">
+      <c r="B15" s="35" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="29" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="29" t="s">
+      <c r="B16" s="35" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="29" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="29" t="s">
+      <c r="B17" s="35" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="29" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="29" t="s">
+      <c r="B18" s="35" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="29" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="29" t="s">
+      <c r="B19" s="35" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="29" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="29" t="s">
+      <c r="B20" s="35" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="31" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="29" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="32" t="s">
         <v>155</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="29" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="29" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="29" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="29" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="29" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="29" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="31" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="32" t="s">
-        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2381,48 +2510,48 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="30" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="31" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="32" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -2452,90 +2581,90 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="29" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="29" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="29" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="29" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="29" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="29" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="29" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="29" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="29" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="29" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="29" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="30" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2546,12 +2675,12 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="31" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="32" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2600,191 +2729,191 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D2"/>
     </row>
     <row r="3" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="29" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="B3" s="26"/>
       <c r="C3" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="D3" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B4" s="26"/>
       <c r="C4" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="D4" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B5" s="26"/>
       <c r="C5" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="D5" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6" s="26"/>
       <c r="C6" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D6" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="27" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="B7" s="26"/>
       <c r="C7" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="D7" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="27" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B8" s="26"/>
       <c r="C8" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="D8" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="29" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="B9" s="26"/>
       <c r="C9" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="D9" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="29" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B10" s="26"/>
       <c r="C10" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="D10"/>
     </row>
     <row r="11" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="29" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B11" s="26"/>
       <c r="C11" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="D11"/>
     </row>
     <row r="12" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="29" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="B12" s="26"/>
       <c r="C12" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="D12"/>
     </row>
     <row r="13" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="29" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B13" s="26"/>
       <c r="C13" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="D13" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="29" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="B14" s="26"/>
       <c r="C14" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="D14" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="29" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="B15" s="26"/>
       <c r="C15" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="D15"/>
     </row>
     <row r="16" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="29" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="B16" s="26"/>
       <c r="C16" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="D16"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="31" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C22" s="26"/>
     </row>

</xml_diff>

<commit_message>
fix typo in metadata
</commit_message>
<xml_diff>
--- a/automation/abstimmungsergebnisse/politik_abstimmungen_seit1933_metadata.xlsx
+++ b/automation/abstimmungsergebnisse/politik_abstimmungen_seit1933_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sszgua\Python\git\opendatazurich.github.io\automation\abstimmungsergebnisse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFEEDF6-4D3F-4169-A753-3BE7EC82E898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D236580D-F197-4C0B-AC88-65FD48449C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="-120" windowWidth="27900" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="243">
   <si>
     <t>Tagname</t>
   </si>
@@ -111,9 +111,6 @@
   </si>
   <si>
     <t>Datenlieferant</t>
-  </si>
-  <si>
-    <t>Statistik Stadt Zürich, Präsidialdepartement.</t>
   </si>
   <si>
     <t>Wer ist der Datenlieferant?</t>
@@ -1395,7 +1392,7 @@
   <dimension ref="A1:G68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="255.5" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1463,7 +1460,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="8" t="s">
@@ -1481,7 +1478,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7" t="s">
@@ -1533,191 +1530,191 @@
         <v>9</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>30</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>31</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="14" t="s">
         <v>34</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>35</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>38</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>39</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>20</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>42</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>43</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>20</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="14" t="s">
         <v>46</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>47</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>20</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="14" t="s">
         <v>50</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>51</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>54</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>55</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="14" t="s">
         <v>58</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>59</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="14" t="s">
         <v>62</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>63</v>
       </c>
       <c r="C16" s="17" t="s">
         <v>20</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="14" t="s">
         <v>66</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>67</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>20</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -1729,10 +1726,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>70</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>71</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>20</v>
@@ -1745,32 +1742,32 @@
         <v>8</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="21" t="s">
+      <c r="C21" s="21" t="s">
         <v>73</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="42.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B22" s="21"/>
       <c r="C22" s="21"/>
       <c r="D22" s="1"/>
       <c r="E22" s="7"/>
       <c r="F22" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
@@ -1779,7 +1776,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="7"/>
       <c r="F23" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1804,10 +1801,10 @@
     </row>
     <row r="27" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" s="9" t="s">
         <v>77</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>78</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>9</v>
@@ -1815,288 +1812,288 @@
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
       <c r="B28" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="D28" s="13" t="s">
         <v>81</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>82</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="B29" s="21" t="s">
+      <c r="C29" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="C29" s="21" t="s">
+      <c r="D29" s="21" t="s">
         <v>86</v>
-      </c>
-      <c r="D29" s="21" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B30" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="C30" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="D30" s="21" t="s">
         <v>89</v>
-      </c>
-      <c r="D30" s="21" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B31" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="C31" s="21" t="s">
+      <c r="D31" s="21" t="s">
         <v>92</v>
-      </c>
-      <c r="D31" s="21" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B32" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="D32" s="21" t="s">
         <v>95</v>
-      </c>
-      <c r="D32" s="21" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B33" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="C33" s="21" t="s">
+      <c r="D33" s="21" t="s">
         <v>98</v>
-      </c>
-      <c r="D33" s="21" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B34" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="C34" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C34" s="21" t="s">
+      <c r="D34" s="21" t="s">
         <v>101</v>
-      </c>
-      <c r="D34" s="21" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B35" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="C35" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="C35" s="21" t="s">
+      <c r="D35" s="21" t="s">
         <v>104</v>
-      </c>
-      <c r="D35" s="21" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B36" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="C36" s="21" t="s">
+      <c r="D36" s="21" t="s">
         <v>107</v>
-      </c>
-      <c r="D36" s="21" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B37" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="C37" s="21" t="s">
+      <c r="D37" s="21" t="s">
         <v>110</v>
-      </c>
-      <c r="D37" s="21" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C38" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="D38" s="21" t="s">
         <v>112</v>
-      </c>
-      <c r="D38" s="21" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C39" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="D39" s="21" t="s">
         <v>114</v>
-      </c>
-      <c r="D39" s="21" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C41" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="D41" s="21" t="s">
         <v>117</v>
-      </c>
-      <c r="D41" s="21" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C42" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="D42" s="21" t="s">
         <v>119</v>
-      </c>
-      <c r="D42" s="21" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C43" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D43" s="21" t="s">
         <v>121</v>
-      </c>
-      <c r="D43" s="21" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C44" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="D44" s="21" t="s">
         <v>123</v>
-      </c>
-      <c r="D44" s="21" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="45" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B45" s="21"/>
       <c r="C45" s="21"/>
       <c r="D45" s="21"/>
       <c r="E45" s="7"/>
       <c r="F45" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="4" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B46" s="21"/>
       <c r="C46" s="21"/>
       <c r="D46" s="21"/>
       <c r="E46" s="7"/>
       <c r="F46" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B47" s="21"/>
       <c r="C47" s="21"/>
       <c r="D47" s="21"/>
       <c r="E47" s="7"/>
       <c r="F47" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B48" s="21"/>
       <c r="C48" s="21"/>
@@ -2105,7 +2102,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B49" s="21"/>
       <c r="C49" s="21"/>
@@ -2114,7 +2111,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B50" s="21"/>
       <c r="C50" s="21"/>
@@ -2123,7 +2120,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B51" s="21"/>
       <c r="C51" s="21"/>
@@ -2132,7 +2129,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B52" s="21"/>
       <c r="C52" s="21"/>
@@ -2141,7 +2138,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B53" s="21"/>
       <c r="C53" s="21"/>
@@ -2150,7 +2147,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B54" s="21"/>
       <c r="C54" s="21"/>
@@ -2159,7 +2156,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B55" s="21"/>
       <c r="C55" s="21"/>
@@ -2168,7 +2165,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B56" s="21"/>
       <c r="C56" s="21"/>
@@ -2177,7 +2174,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B57" s="21"/>
       <c r="C57" s="21"/>
@@ -2186,7 +2183,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B58" s="21"/>
       <c r="C58" s="21"/>
@@ -2213,7 +2210,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B62" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="7"/>
@@ -2227,10 +2224,10 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B64" s="9" t="s">
         <v>129</v>
-      </c>
-      <c r="B64" s="9" t="s">
-        <v>130</v>
       </c>
       <c r="C64" s="9" t="s">
         <v>20</v>
@@ -2241,7 +2238,7 @@
     </row>
     <row r="65" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B65" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C65" s="13" t="s">
         <v>12</v>
@@ -2249,12 +2246,12 @@
       <c r="D65" s="13"/>
       <c r="E65" s="7"/>
       <c r="F65" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B66" s="12"/>
       <c r="C66" s="12"/>
@@ -2264,7 +2261,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B67" s="12"/>
       <c r="C67" s="12"/>
@@ -2315,172 +2312,172 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="29" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="29" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="29" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="29" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B11" s="35" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="29" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B12" s="35" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B13" s="35" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="29" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B14" s="35" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="29" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B15" s="35" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="29" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B16" s="35" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B17" s="35" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="29" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B18" s="35" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="29" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B19" s="35" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="29" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B20" s="35" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="32" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -2510,48 +2507,48 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="30" t="s">
+        <v>159</v>
+      </c>
+      <c r="C6" s="24" t="s">
         <v>160</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="32" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -2581,90 +2578,90 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="29" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="29" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="29" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="29" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="30" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2675,12 +2672,12 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="32" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2729,191 +2726,191 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C1" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="D1" s="28" t="s">
         <v>176</v>
-      </c>
-      <c r="D1" s="28" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D2"/>
     </row>
     <row r="3" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B3" s="26"/>
       <c r="C3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D3" t="s">
         <v>181</v>
-      </c>
-      <c r="D3" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B4" s="26"/>
       <c r="C4" t="s">
+        <v>183</v>
+      </c>
+      <c r="D4" t="s">
         <v>184</v>
-      </c>
-      <c r="D4" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B5" s="26"/>
       <c r="C5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D5" t="s">
         <v>187</v>
-      </c>
-      <c r="D5" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" s="26"/>
       <c r="C6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D6" t="s">
         <v>189</v>
-      </c>
-      <c r="D6" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B7" s="26"/>
       <c r="C7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D7" t="s">
         <v>192</v>
-      </c>
-      <c r="D7" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="27" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B8" s="26"/>
       <c r="C8" t="s">
+        <v>194</v>
+      </c>
+      <c r="D8" t="s">
         <v>195</v>
-      </c>
-      <c r="D8" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="29" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B9" s="26"/>
       <c r="C9" t="s">
+        <v>197</v>
+      </c>
+      <c r="D9" t="s">
         <v>198</v>
-      </c>
-      <c r="D9" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="29" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B10" s="26"/>
       <c r="C10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D10"/>
     </row>
     <row r="11" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B11" s="26"/>
       <c r="C11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D11"/>
     </row>
     <row r="12" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B12" s="26"/>
       <c r="C12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D12"/>
     </row>
     <row r="13" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B13" s="26"/>
       <c r="C13" t="s">
+        <v>206</v>
+      </c>
+      <c r="D13" t="s">
         <v>207</v>
-      </c>
-      <c r="D13" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="29" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B14" s="26"/>
       <c r="C14" t="s">
+        <v>209</v>
+      </c>
+      <c r="D14" t="s">
         <v>210</v>
-      </c>
-      <c r="D14" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="29" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B15" s="26"/>
       <c r="C15" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D15"/>
     </row>
     <row r="16" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="29" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B16" s="26"/>
       <c r="C16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D16"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C22" s="26"/>
     </row>

</xml_diff>